<commit_message>
Updated documentation for phase 3
This includes the latest files for documentation in the last 30 mins of the project.
</commit_message>
<xml_diff>
--- a/Phase3/Copy of Gantt chart.xlsx
+++ b/Phase3/Copy of Gantt chart.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="102">
   <si>
     <t>GROUP 3 BLACKJACK GANTT CHART</t>
   </si>
@@ -4275,7 +4275,7 @@
         <v>12</v>
       </c>
       <c r="H43" s="63">
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="I43" s="102"/>
       <c r="J43" s="103"/>
@@ -4352,7 +4352,7 @@
         <v>12</v>
       </c>
       <c r="H44" s="63">
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="I44" s="102"/>
       <c r="J44" s="103"/>
@@ -4429,7 +4429,7 @@
         <v>12</v>
       </c>
       <c r="H45" s="63">
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="I45" s="102"/>
       <c r="J45" s="103"/>
@@ -4506,7 +4506,7 @@
         <v>12</v>
       </c>
       <c r="H46" s="63">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I46" s="102"/>
       <c r="J46" s="103"/>
@@ -4583,7 +4583,7 @@
         <v>12</v>
       </c>
       <c r="H47" s="63">
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="I47" s="102"/>
       <c r="J47" s="103"/>
@@ -4649,13 +4649,19 @@
       <c r="D48" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
+      <c r="E48" s="61">
+        <v>45598.0</v>
+      </c>
+      <c r="F48" s="61">
+        <v>45610.0</v>
+      </c>
       <c r="G48" s="106">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H48" s="63"/>
+        <v>12</v>
+      </c>
+      <c r="H48" s="63">
+        <v>0.8</v>
+      </c>
       <c r="I48" s="93"/>
       <c r="J48" s="94"/>
       <c r="K48" s="95"/>
@@ -4720,13 +4726,19 @@
       <c r="D49" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
+      <c r="E49" s="61">
+        <v>45599.0</v>
+      </c>
+      <c r="F49" s="61">
+        <v>45611.0</v>
+      </c>
       <c r="G49" s="106">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H49" s="63"/>
+        <v>12</v>
+      </c>
+      <c r="H49" s="63">
+        <v>0.8</v>
+      </c>
       <c r="I49" s="93"/>
       <c r="J49" s="94"/>
       <c r="K49" s="95"/>
@@ -4802,7 +4814,7 @@
         <v>10</v>
       </c>
       <c r="H50" s="63">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I50" s="93"/>
       <c r="J50" s="94"/>
@@ -4868,13 +4880,19 @@
       <c r="D51" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
+      <c r="E51" s="61">
+        <v>45622.0</v>
+      </c>
+      <c r="F51" s="61">
+        <v>45632.0</v>
+      </c>
       <c r="G51" s="106">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H51" s="63"/>
+        <v>10</v>
+      </c>
+      <c r="H51" s="63">
+        <v>1.0</v>
+      </c>
       <c r="I51" s="93"/>
       <c r="J51" s="94"/>
       <c r="K51" s="95"/>
@@ -5103,7 +5121,9 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="H54" s="63"/>
+      <c r="H54" s="63">
+        <v>1.0</v>
+      </c>
       <c r="I54" s="93"/>
       <c r="J54" s="94"/>
       <c r="K54" s="95"/>
@@ -5165,14 +5185,22 @@
       <c r="C55" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="60"/>
-      <c r="E55" s="61"/>
-      <c r="F55" s="61"/>
+      <c r="D55" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" s="61">
+        <v>45623.0</v>
+      </c>
+      <c r="F55" s="61">
+        <v>45630.0</v>
+      </c>
       <c r="G55" s="106">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H55" s="63"/>
+        <v>7</v>
+      </c>
+      <c r="H55" s="63">
+        <v>1.0</v>
+      </c>
       <c r="I55" s="93"/>
       <c r="J55" s="94"/>
       <c r="K55" s="95"/>
@@ -5237,13 +5265,19 @@
       <c r="D56" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="E56" s="61"/>
-      <c r="F56" s="61"/>
+      <c r="E56" s="61">
+        <v>45624.0</v>
+      </c>
+      <c r="F56" s="61">
+        <v>45631.0</v>
+      </c>
       <c r="G56" s="106">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H56" s="63"/>
+        <v>7</v>
+      </c>
+      <c r="H56" s="63">
+        <v>1.0</v>
+      </c>
       <c r="I56" s="93"/>
       <c r="J56" s="94"/>
       <c r="K56" s="95"/>
@@ -5306,15 +5340,21 @@
         <v>96</v>
       </c>
       <c r="D57" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="E57" s="61"/>
-      <c r="F57" s="61"/>
+        <v>71</v>
+      </c>
+      <c r="E57" s="61">
+        <v>45625.0</v>
+      </c>
+      <c r="F57" s="61">
+        <v>45632.0</v>
+      </c>
       <c r="G57" s="106">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H57" s="63"/>
+        <v>7</v>
+      </c>
+      <c r="H57" s="63">
+        <v>1.0</v>
+      </c>
       <c r="I57" s="93"/>
       <c r="J57" s="94"/>
       <c r="K57" s="95"/>
@@ -5389,7 +5429,9 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="H58" s="63"/>
+      <c r="H58" s="63">
+        <v>1.0</v>
+      </c>
       <c r="I58" s="93"/>
       <c r="J58" s="94"/>
       <c r="K58" s="95"/>
@@ -5451,14 +5493,22 @@
       <c r="C59" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="D59" s="60"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
+      <c r="D59" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="E59" s="61">
+        <v>45623.0</v>
+      </c>
+      <c r="F59" s="61">
+        <v>45629.0</v>
+      </c>
       <c r="G59" s="106">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H59" s="63"/>
+        <v>6</v>
+      </c>
+      <c r="H59" s="63">
+        <v>1.0</v>
+      </c>
       <c r="I59" s="93"/>
       <c r="J59" s="94"/>
       <c r="K59" s="95"/>
@@ -5520,7 +5570,9 @@
       <c r="C60" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="D60" s="60"/>
+      <c r="D60" s="60" t="s">
+        <v>37</v>
+      </c>
       <c r="E60" s="61">
         <v>45621.0</v>
       </c>
@@ -5532,7 +5584,7 @@
         <v>10</v>
       </c>
       <c r="H60" s="63">
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="I60" s="102"/>
       <c r="J60" s="103"/>
@@ -5595,7 +5647,9 @@
       <c r="C61" s="110" t="s">
         <v>100</v>
       </c>
-      <c r="D61" s="60"/>
+      <c r="D61" s="60" t="s">
+        <v>37</v>
+      </c>
       <c r="E61" s="61"/>
       <c r="F61" s="61"/>
       <c r="G61" s="106"/>
@@ -5646,18 +5700,16 @@
       <c r="AZ61" s="71"/>
       <c r="BA61" s="71"/>
       <c r="BB61" s="70"/>
-      <c r="BC61" s="107"/>
-      <c r="BD61" s="107"/>
-      <c r="BE61" s="107"/>
-      <c r="BF61" s="107"/>
+      <c r="BC61" s="70"/>
+      <c r="BD61" s="70"/>
+      <c r="BE61" s="70"/>
+      <c r="BF61" s="70"/>
       <c r="BG61" s="58"/>
       <c r="BH61" s="58"/>
     </row>
     <row r="62" ht="17.25" customHeight="1" outlineLevel="1">
       <c r="A62" s="58"/>
-      <c r="B62" s="59">
-        <v>5.50000000000005</v>
-      </c>
+      <c r="B62" s="59"/>
       <c r="C62" s="60"/>
       <c r="D62" s="60" t="s">
         <v>101</v>

</xml_diff>